<commit_message>
adding data on what people by with SNAP
</commit_message>
<xml_diff>
--- a/reports/charts.xlsx
+++ b/reports/charts.xlsx
@@ -8,55 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelvnguemaha/repos/cmsdatajam/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9E6979-53B2-8043-85B0-684CBA760E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646B9CDC-9B49-F943-83E2-B0C42BEC8748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36700" yWindow="720" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{EB6B0780-E583-A149-8CD4-1CC416B72D70}"/>
+    <workbookView xWindow="0" yWindow="1140" windowWidth="30240" windowHeight="17860" activeTab="4" xr2:uid="{EB6B0780-E583-A149-8CD4-1CC416B72D70}"/>
   </bookViews>
   <sheets>
     <sheet name="CKD Incidence Research" sheetId="4" r:id="rId1"/>
     <sheet name="Diet Followed" sheetId="3" r:id="rId2"/>
-    <sheet name="Reasons for Diets" sheetId="2" r:id="rId3"/>
-    <sheet name="Money for Food" sheetId="1" r:id="rId4"/>
+    <sheet name="Money for Food" sheetId="1" r:id="rId3"/>
+    <sheet name="Reasons for Diets" sheetId="2" r:id="rId4"/>
+    <sheet name="What SNAP People Buy" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.10" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'Money for Food'!$B$1</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'Money for Food'!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Money for Food'!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'What SNAP People Buy'!$A$2:$A$31</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'What SNAP People Buy'!$D$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'What SNAP People Buy'!$D$2:$D$31</definedName>
     <definedName name="_xlchart.v2.0" hidden="1">'Diet Followed'!$A$2:$A$20</definedName>
     <definedName name="_xlchart.v2.1" hidden="1">'Diet Followed'!$B$1</definedName>
     <definedName name="_xlchart.v2.2" hidden="1">'Diet Followed'!$B$2:$B$20</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Diet Followed'!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'Diet Followed'!$B$1</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">'Diet Followed'!$B$2:$B$20</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">'Reasons for Diets'!$A$2:$A$11</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">'Reasons for Diets'!$B$1</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">'Reasons for Diets'!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Reasons for Diets'!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'Reasons for Diets'!$B$1</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'Reasons for Diets'!$B$2:$B$11</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Frequency</t>
   </si>
@@ -227,13 +201,128 @@
   </si>
   <si>
     <t>Source (Table 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meat, Poultry and Seafood </t>
+  </si>
+  <si>
+    <t>Prepared Desserts</t>
+  </si>
+  <si>
+    <t>Bread and Crackers</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Prepared Foods</t>
+  </si>
+  <si>
+    <t>Condiments and Seasoning</t>
+  </si>
+  <si>
+    <t>Candy</t>
+  </si>
+  <si>
+    <t>Juices</t>
+  </si>
+  <si>
+    <t>Bottled Water</t>
+  </si>
+  <si>
+    <t>Other Dairy Products</t>
+  </si>
+  <si>
+    <t>Soups</t>
+  </si>
+  <si>
+    <t>Nuts and Seeds</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Flour and Prepared Flour Mixes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweetened Beverages </t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Frozen Prepared Foods</t>
+  </si>
+  <si>
+    <t>High Fat Dairy/Cheese</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Salty Snacks</t>
+  </si>
+  <si>
+    <t>Cereal</t>
+  </si>
+  <si>
+    <t>Fats and Oils</t>
+  </si>
+  <si>
+    <t>Baby Food</t>
+  </si>
+  <si>
+    <t>Coffee and Tea</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Pasta, Other Cereal Products</t>
+  </si>
+  <si>
+    <t>Sugars</t>
+  </si>
+  <si>
+    <t>Beans</t>
+  </si>
+  <si>
+    <t>Jams, Jellies, and Other Sweets</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Food Category</t>
+  </si>
+  <si>
+    <t>SNAP</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Percentage of Total Spend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source </t>
+  </si>
+  <si>
+    <t>https://www.fns.usda.gov/snap/foods-typically-purchased-supplemental-nutrition-assistance-program-snap-households</t>
+  </si>
+  <si>
+    <t>Total Summary Category Expenditures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,8 +360,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="TimesNewRomanPSMT"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +376,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,12 +399,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,6 +1159,434 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'What SNAP People Buy'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Total Spend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'What SNAP People Buy'!$A$2:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>Meat, Poultry and Seafood </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sweetened Beverages </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Vegetables</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Frozen Prepared Foods</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Prepared Desserts</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>High Fat Dairy/Cheese</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bread and Crackers</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Fruits</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Milk</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Salty Snacks</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Prepared Foods</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Cereal</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Condiments and Seasoning</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Fats and Oils</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Candy</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Baby Food</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Juices</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Coffee and Tea</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Bottled Water</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Eggs</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Other Dairy Products</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Pasta, Other Cereal Products</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Soups</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Sugars</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Nuts and Seeds</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Beans</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Rice</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Jams, Jellies, and Other Sweets</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Flour and Prepared Flour Mixes</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Miscellaneous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'What SNAP People Buy'!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.19191550794012613</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2500569865511736E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1939822201960324E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.917407491831927E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8961325127269962E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5010257579211306E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3932072031000672E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6835346858141468E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5362054555124985E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4283109186232043E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0727148392979253E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8402097105083197E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6532938226578522E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.356963756553453E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.10014436592964E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9269052503609146E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6776840665602918E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2673808981080463E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1868399057822351E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1214953271028035E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0607096725172857E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0090418661195958E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.5281513562799174E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.2546159106450861E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.0844920598738684E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.8202264265633302E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.5741205075602153E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.422156371096421E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8417293518729573E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8265329382265785E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B9E7-2C4E-8BD5-8A9BB9183F3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1436413327"/>
+        <c:axId val="440051535"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1436413327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440051535"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="440051535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1436413327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
@@ -1117,7 +1650,7 @@
           <cx:dataId val="0"/>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="1">
+      <cx:axis id="0">
         <cx:catScaling gapWidth="0.0599999987"/>
         <cx:tickLabels/>
       </cx:axis>
@@ -1131,10 +1664,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v2.6</cx:f>
+        <cx:f>_xlchart.v2.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v2.8</cx:f>
+        <cx:f>_xlchart.v2.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1172,7 +1705,7 @@
         <cx:series layoutId="funnel" uniqueId="{5A3273E7-578B-B949-8958-394540F0D41A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v2.7</cx:f>
+              <cx:f>_xlchart.v2.4</cx:f>
               <cx:v>Percentage of People</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1196,7 +1729,7 @@
           <cx:dataId val="0"/>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="1">
+      <cx:axis id="0">
         <cx:catScaling gapWidth="0.0599999987"/>
         <cx:tickLabels/>
         <cx:txPr>
@@ -1383,6 +1916,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2408,6 +2981,511 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="419">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2915,7 +3993,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3548,6 +4626,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF6AD54-5B80-5176-DDEF-7DCCD8A5DE5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -3627,27 +4746,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF6AD54-5B80-5176-DDEF-7DCCD8A5DE5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA98E290-7997-BB05-5085-EF2CD2E846B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3971,13 +5090,13 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -3985,7 +5104,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3993,7 +5112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4001,7 +5120,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4009,7 +5128,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4017,7 +5136,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4025,7 +5144,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:6">
       <c r="E17" s="4" t="s">
         <v>46</v>
       </c>
@@ -4044,16 +5163,16 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection sqref="A1:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -4061,7 +5180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4069,7 +5188,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4077,7 +5196,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -4085,7 +5204,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4093,7 +5212,7 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4101,7 +5220,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -4109,7 +5228,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -4117,7 +5236,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -4125,7 +5244,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -4133,7 +5252,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -4141,7 +5260,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -4149,7 +5268,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -4157,7 +5276,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -4165,7 +5284,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -4173,7 +5292,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -4181,7 +5300,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -4189,7 +5308,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -4197,7 +5316,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -4205,7 +5324,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -4213,7 +5332,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="D29" s="4" t="s">
         <v>45</v>
       </c>
@@ -4228,6 +5347,82 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF792B-88E2-BB42-A41A-395D3BE286EC}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7">
+      <c r="F28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179C0B42-A04F-774E-A6D7-2E5D6FB9BAE6}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -4235,13 +5430,13 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -4249,7 +5444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4257,7 +5452,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4265,7 +5460,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -4273,7 +5468,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4281,7 +5476,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -4289,7 +5484,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4297,7 +5492,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4305,7 +5500,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4313,7 +5508,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4321,7 +5516,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4329,17 +5524,17 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:5">
       <c r="D19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:5">
       <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:5">
       <c r="D22" s="4" t="s">
         <v>45</v>
       </c>
@@ -4353,74 +5548,503 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF792B-88E2-BB42-A41A-395D3BE286EC}">
-  <dimension ref="A1:G28"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B49EC61-3B3E-5946-B385-0A338875A3FD}">
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="1" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" s="8">
+        <v>1262.9000000000001</v>
+      </c>
+      <c r="D2" s="9">
+        <f>C2/C$32</f>
+        <v>0.19191550794012613</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" s="8">
+        <v>608.70000000000005</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D32" si="0">C3/C$32</f>
+        <v>9.2500569865511736E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" s="8">
+        <v>473.4</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>7.1939822201960324E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="5">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C5" s="8">
+        <v>455.2</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>6.917407491831927E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="5">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C6" s="8">
+        <v>453.8</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>6.8961325127269962E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="5">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F28" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>48</v>
+      <c r="C7" s="8">
+        <v>427.8</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5010257579211306E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8">
+        <v>354.9</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>5.3932072031000672E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8">
+        <v>308.2</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>4.6835346858141468E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8">
+        <v>232.7</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>3.5362054555124985E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8">
+        <v>225.6</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>3.4283109186232043E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="5">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8">
+        <v>202.2</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>3.0727148392979253E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8">
+        <v>186.9</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>2.8402097105083197E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5">
+        <v>13</v>
+      </c>
+      <c r="C14" s="8">
+        <v>174.6</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>2.6532938226578522E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="5">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8">
+        <v>155.1</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="0"/>
+        <v>2.356963756553453E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="5">
+        <v>15</v>
+      </c>
+      <c r="C16" s="8">
+        <v>138.19999999999999</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
+        <v>2.10014436592964E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="5">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8">
+        <v>126.8</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9269052503609146E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="5">
+        <v>17</v>
+      </c>
+      <c r="C18" s="8">
+        <v>110.4</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
+        <v>1.6776840665602918E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8">
+        <v>83.4</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2673808981080463E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="5">
+        <v>19</v>
+      </c>
+      <c r="C20" s="8">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1868399057822351E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20</v>
+      </c>
+      <c r="C21" s="8">
+        <v>73.8</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1214953271028035E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="5">
+        <v>21</v>
+      </c>
+      <c r="C22" s="8">
+        <v>69.8</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0607096725172857E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="5">
+        <v>22</v>
+      </c>
+      <c r="C23" s="8">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0090418661195958E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5">
+        <v>23</v>
+      </c>
+      <c r="C24" s="8">
+        <v>62.7</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="0"/>
+        <v>9.5281513562799174E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="5">
+        <v>24</v>
+      </c>
+      <c r="C25" s="8">
+        <v>60.9</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="0"/>
+        <v>9.2546159106450861E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="5">
+        <v>25</v>
+      </c>
+      <c r="C26" s="8">
+        <v>53.2</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="0"/>
+        <v>8.0844920598738684E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="5">
+        <v>26</v>
+      </c>
+      <c r="C27" s="8">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="0"/>
+        <v>5.8202264265633302E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="5">
+        <v>27</v>
+      </c>
+      <c r="C28" s="8">
+        <v>30.1</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5741205075602153E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="5">
+        <v>28</v>
+      </c>
+      <c r="C29" s="8">
+        <v>29.1</v>
+      </c>
+      <c r="D29" s="9">
+        <f t="shared" si="0"/>
+        <v>4.422156371096421E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="5">
+        <v>29</v>
+      </c>
+      <c r="C30" s="8">
+        <v>18.7</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="0"/>
+        <v>2.8417293518729573E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="5">
+        <v>30</v>
+      </c>
+      <c r="C31" s="8">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D31" s="9">
+        <f t="shared" si="0"/>
+        <v>2.8265329382265785E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="7">
+        <f>SUM(C2:C31)</f>
+        <v>6580.5000000000009</v>
+      </c>
+      <c r="D32" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>